<commit_message>
Ahora busca tanto en mayusculas como en minusculas
</commit_message>
<xml_diff>
--- a/test_folder/file10.xlsx
+++ b/test_folder/file10.xlsx
@@ -22,7 +22,7 @@
     <t>num</t>
   </si>
   <si>
-    <t>upb401</t>
+    <t>uPB401</t>
   </si>
   <si>
     <t>upb402</t>
@@ -33,7 +33,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -44,6 +44,12 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -77,10 +83,10 @@
   </cellStyleXfs>
   <cellXfs count="4">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
@@ -406,7 +412,7 @@
         <v>1</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -414,7 +420,7 @@
         <v>78</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
@@ -422,7 +428,7 @@
         <v>126</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
       <c r="A4" s="2">
         <v>403</v>
       </c>
@@ -430,7 +436,7 @@
         <v>70</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
       <c r="A5" s="2">
         <v>404</v>
       </c>
@@ -438,7 +444,7 @@
         <v>173</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
       <c r="A6" s="2">
         <v>405</v>
       </c>
@@ -446,7 +452,7 @@
         <v>195</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
       <c r="A7" s="2">
         <v>406</v>
       </c>
@@ -454,7 +460,7 @@
         <v>202</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
       <c r="A8" s="2">
         <v>407</v>
       </c>
@@ -462,7 +468,7 @@
         <v>219</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
       <c r="A9" s="2">
         <v>408</v>
       </c>
@@ -470,7 +476,7 @@
         <v>188</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
       <c r="A10" s="2">
         <v>409</v>
       </c>
@@ -478,7 +484,7 @@
         <v>112</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5">
       <c r="A11" s="2">
         <v>410</v>
       </c>
@@ -486,7 +492,7 @@
         <v>221</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5">
       <c r="A12" s="2">
         <v>411</v>
       </c>

</xml_diff>